<commit_message>
UC time table updated
</commit_message>
<xml_diff>
--- a/documentation/useCases/TimeEstimationUC.xlsx
+++ b/documentation/useCases/TimeEstimationUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\useCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5F332D-2EAF-4259-9744-E16BFD4823AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0700B1C-74A9-410A-A738-2E3106EE76FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Time spent on use cases</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://perfecttime.myjetbrains.com/youtrack/reports/time/145-1 </t>
+  </si>
+  <si>
+    <t>(copy and export are separat use cases, but tasks often do affect both, which is why they are put together for time evaluation)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,6 +618,7 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -719,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -733,6 +737,9 @@
       <c r="H12" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time/FP diagram and calculation added
</commit_message>
<xml_diff>
--- a/documentation/useCases/TimeEstimationUC.xlsx
+++ b/documentation/useCases/TimeEstimationUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\useCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0700B1C-74A9-410A-A738-2E3106EE76FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180D282-E3E5-46F7-A569-F456BA34242C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Time spent on use cases</t>
   </si>
@@ -98,6 +98,33 @@
   </si>
   <si>
     <t>(copy and export are separat use cases, but tasks often do affect both, which is why they are put together for time evaluation)</t>
+  </si>
+  <si>
+    <t>(view all trips and CRUD trips are separat use cases, but tasks often  affect both, which is why they are put together for time evaluation)</t>
+  </si>
+  <si>
+    <t>Time/FP</t>
+  </si>
+  <si>
+    <t>Time Total (/wo warm-up)</t>
+  </si>
+  <si>
+    <t>Total Semester 1</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>Schätzungen</t>
+  </si>
+  <si>
+    <t>Time (estimated)</t>
+  </si>
+  <si>
+    <t>Time-FP-Evaluation</t>
+  </si>
+  <si>
+    <t>Total Semester 2</t>
   </si>
 </sst>
 </file>
@@ -152,11 +179,122 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -165,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -173,12 +311,131 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -210,8 +467,1121 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time Total (without warm-up)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>UC!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time Total (/wo warm-up)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="15"/>
+            <c:backward val="28"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>UC!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>UC!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F705-4BE6-B6A1-6298B44A35A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="427835248"/>
+        <c:axId val="427838200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="427835248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Function Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427838200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="427838200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in h</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427835248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93E79EFF-E94F-4670-96A6-EF95CB37DE2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86A4CECC-2922-4D2A-9955-EA7E9D220A37}" name="Tabelle1" displayName="Tabelle1" ref="A6:I12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86A4CECC-2922-4D2A-9955-EA7E9D220A37}" name="Tabelle1" displayName="Tabelle1" ref="A6:I12" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A6:I12" xr:uid="{5C67A54D-222E-4FF5-9573-520223123106}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{601B8A81-A423-4342-9310-3B039E150F63}" name="UC "/>
@@ -227,6 +1597,39 @@
       <calculatedColumnFormula>FALSE</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{947A6D29-0BC8-443D-A656-5CF90ED82879}" name="Remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7531F48-F369-427D-BF0E-B373BD3D9464}" name="Tabelle2" displayName="Tabelle2" ref="A16:D21" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A16:D21" xr:uid="{5C48C029-3835-4A93-A46E-44532C92FAA3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0447BFA7-3026-4AF7-A1B7-18AE0CFBF124}" name="UC" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A2FB336A-5D1A-465E-8C03-AD6268938476}" name="FP" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{AB75E940-54C0-4B8B-9EA7-F80E0F712E4D}" name="Time Total (/wo warm-up)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E3D2115D-CD04-4BCA-BD7D-98B341DA5312}" name="Time/FP" dataDxfId="0">
+      <calculatedColumnFormula>C17/B17</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B577A4E0-9391-4DF9-99B0-11B059EFA638}" name="Tabelle3" displayName="Tabelle3" ref="A23:C26" totalsRowShown="0">
+  <autoFilter ref="A23:C26" xr:uid="{9A2F3DE4-4BA2-4301-84EB-47561E8B86BA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D8456900-3670-4449-B566-12566F1FF919}" name="Schätzungen">
+      <calculatedColumnFormula>A11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{DC988EF7-EB92-44C5-97D8-A22603824293}" name="FP">
+      <calculatedColumnFormula>G11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{19E74BDF-4684-4720-8463-4DBCA47C7700}" name="Time (estimated)">
+      <calculatedColumnFormula>0.2558*B24+9.3956</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -529,16 +1932,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142AC939-646A-4C14-B811-03896D9CEEB5}">
-  <dimension ref="A2:I12"/>
+  <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="46.140625" customWidth="1"/>
@@ -614,13 +2018,16 @@
         <f>SUM(B7:E7)</f>
         <v>15</v>
       </c>
+      <c r="G7">
+        <v>29.44</v>
+      </c>
       <c r="H7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -640,9 +2047,16 @@
         <f t="shared" ref="F8:F12" si="0">SUM(B8:E8)</f>
         <v>32</v>
       </c>
+      <c r="G8">
+        <f>88.23+10.68</f>
+        <v>98.91</v>
+      </c>
       <c r="H8" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,6 +2079,10 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
+      <c r="G9">
+        <f>37.72*2</f>
+        <v>75.44</v>
+      </c>
       <c r="H9" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -693,6 +2111,10 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
+      <c r="G10">
+        <f>37.72*2</f>
+        <v>75.44</v>
+      </c>
       <c r="H10" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -718,6 +2140,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="G11">
+        <v>42.32</v>
+      </c>
       <c r="H11" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -734,12 +2159,176 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G12">
+        <f>34.2*2</f>
+        <v>68.400000000000006</v>
+      </c>
       <c r="H12" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="str">
+        <f>A7</f>
+        <v>UC Register / Login</v>
+      </c>
+      <c r="B17" s="5">
+        <f>G7</f>
+        <v>29.44</v>
+      </c>
+      <c r="C17" s="5">
+        <f>SUM(B7:D7)</f>
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <f>C17/B17</f>
+        <v>0.44157608695652173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="str">
+        <f t="shared" ref="A18:A20" si="1">A8</f>
+        <v>UC CRUD trips</v>
+      </c>
+      <c r="B18" s="5">
+        <f>G8</f>
+        <v>98.91</v>
+      </c>
+      <c r="C18" s="5">
+        <f>SUM(B8:D8)</f>
+        <v>27</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" ref="D18:D21" si="2">C18/B18</f>
+        <v>0.27297543221110099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>UC CRUD locations</v>
+      </c>
+      <c r="B19" s="5">
+        <f>G9</f>
+        <v>75.44</v>
+      </c>
+      <c r="C19" s="5">
+        <f>SUM(B9:D9)</f>
+        <v>46</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="2"/>
+        <v>0.6097560975609756</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>UC CRUD activities</v>
+      </c>
+      <c r="B20" s="5">
+        <f>G10</f>
+        <v>75.44</v>
+      </c>
+      <c r="C20" s="5">
+        <f>SUM(B10:D10)</f>
+        <v>23</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="2"/>
+        <v>0.3048780487804878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="12">
+        <f>SUM(B17:B20)</f>
+        <v>279.23</v>
+      </c>
+      <c r="C21" s="12">
+        <f>SUM(C17:C20)</f>
+        <v>109</v>
+      </c>
+      <c r="D21" s="13">
+        <f t="shared" si="2"/>
+        <v>0.3903592020914658</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>A11</f>
+        <v>UC User Management</v>
+      </c>
+      <c r="B24">
+        <f>G11</f>
+        <v>42.32</v>
+      </c>
+      <c r="C24">
+        <f>0.2558*B24+9.3956</f>
+        <v>20.221056000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>A12</f>
+        <v>UC Export / Copy Trip</v>
+      </c>
+      <c r="B25">
+        <f>G12</f>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="C25">
+        <f>0.2558*B25+9.3956</f>
+        <v>26.892320000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <f>SUM(B24:B25)</f>
+        <v>110.72</v>
+      </c>
+      <c r="C26">
+        <f>SUM(C24:C25)</f>
+        <v>47.113376000000002</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +2336,12 @@
     <hyperlink ref="C4" r:id="rId1" xr:uid="{D1D95D30-F1B5-45CB-BC2A-53B505397567}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated presentation and time calc
</commit_message>
<xml_diff>
--- a/documentation/useCases/TimeEstimationUC.xlsx
+++ b/documentation/useCases/TimeEstimationUC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\useCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821176ED-D902-4300-8C7C-0200B3021CE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B225EF-B26F-4EAE-BBBB-896E6EB486DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
+    <workbookView xWindow="1800" yWindow="2070" windowWidth="15375" windowHeight="7875" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
   </bookViews>
   <sheets>
     <sheet name="UC" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Time spent on use cases</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>UC Export</t>
+  </si>
+  <si>
+    <t>Buffer:</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1621,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B577A4E0-9391-4DF9-99B0-11B059EFA638}" name="Tabelle3" displayName="Tabelle3" ref="A23:C27" totalsRowShown="0">
-  <autoFilter ref="A23:C27" xr:uid="{9A2F3DE4-4BA2-4301-84EB-47561E8B86BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B577A4E0-9391-4DF9-99B0-11B059EFA638}" name="Tabelle3" displayName="Tabelle3" ref="A23:C28" totalsRowShown="0">
+  <autoFilter ref="A23:C28" xr:uid="{9A2F3DE4-4BA2-4301-84EB-47561E8B86BA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D8456900-3670-4449-B566-12566F1FF919}" name="Schätzungen">
       <calculatedColumnFormula>A11</calculatedColumnFormula>
@@ -1932,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142AC939-646A-4C14-B811-03896D9CEEB5}">
-  <dimension ref="A2:I27"/>
+  <dimension ref="A2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,6 +2364,18 @@
         <v>56.508975999999997</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>2.5</v>
+      </c>
+      <c r="C28" s="1">
+        <f>C27*Tabelle3[[#This Row],[FP]]</f>
+        <v>141.27243999999999</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{D1D95D30-F1B5-45CB-BC2A-53B505397567}"/>

</xml_diff>

<commit_message>
Adapted final time values
</commit_message>
<xml_diff>
--- a/documentation/useCases/TimeEstimationUC.xlsx
+++ b/documentation/useCases/TimeEstimationUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\useCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEA7FF7-6AC0-4242-A0B4-11A49DFD71C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DB501-B7EB-434F-92E7-02635D1A870E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
   </bookViews>
@@ -446,6 +446,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -455,128 +458,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -622,18 +509,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -676,11 +551,132 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -688,11 +684,15 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -922,7 +922,7 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1843,42 +1843,42 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86A4CECC-2922-4D2A-9955-EA7E9D220A37}" name="Tabelle1" displayName="Tabelle1" ref="A6:J14" totalsRowCount="1" headerRowDxfId="21">
   <autoFilter ref="A6:J13" xr:uid="{5C67A54D-222E-4FF5-9573-520223123106}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{601B8A81-A423-4342-9310-3B039E150F63}" name="UC " totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{75540AED-3EB3-4F31-941D-D3E841D54080}" name="Documentation " totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{601B8A81-A423-4342-9310-3B039E150F63}" name="UC " totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{75540AED-3EB3-4F31-941D-D3E841D54080}" name="Documentation " totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Tabelle1[Documentation ])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{44742907-8F2C-4FCF-8DEE-61BA7ECA4543}" name="Coding " totalsRowFunction="custom" totalsRowDxfId="17">
+    <tableColumn id="3" xr3:uid="{44742907-8F2C-4FCF-8DEE-61BA7ECA4543}" name="Coding " totalsRowFunction="custom" totalsRowDxfId="7">
       <totalsRowFormula>SUM(Tabelle1[Coding ])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9B438196-2177-438C-A44A-8636E52EF290}" name="Testing " totalsRowFunction="custom" totalsRowDxfId="16">
+    <tableColumn id="4" xr3:uid="{9B438196-2177-438C-A44A-8636E52EF290}" name="Testing " totalsRowFunction="custom" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Tabelle1[Testing ])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B716A9E4-62D3-49AF-9B37-5CC43E74EB72}" name="Warm-Up time" totalsRowFunction="custom" totalsRowDxfId="15">
+    <tableColumn id="5" xr3:uid="{B716A9E4-62D3-49AF-9B37-5CC43E74EB72}" name="Warm-Up time" totalsRowFunction="custom" totalsRowDxfId="5">
       <totalsRowFormula>SUM(Tabelle1[Warm-Up time])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{83B3F74C-E728-456F-AD1D-D2D9CCB1CA9E}" name="Total" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="6" xr3:uid="{83B3F74C-E728-456F-AD1D-D2D9CCB1CA9E}" name="Total" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="4">
       <calculatedColumnFormula>SUM(B7:E7)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Tabelle1[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DD6F7461-5964-4423-A8FF-374449E351FE}" name="FP" totalsRowDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{DBB74D18-542D-4647-9968-E267EA472222}" name="Completed?" totalsRowDxfId="11">
+    <tableColumn id="7" xr3:uid="{DD6F7461-5964-4423-A8FF-374449E351FE}" name="FP" totalsRowDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{DBB74D18-542D-4647-9968-E267EA472222}" name="Completed?" totalsRowDxfId="2">
       <calculatedColumnFormula>FALSE</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{947A6D29-0BC8-443D-A656-5CF90ED82879}" name="Remarks" totalsRowDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{37822F84-BE51-440E-9E33-7057374B8388}" name="Spalte1" totalsRowDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{947A6D29-0BC8-443D-A656-5CF90ED82879}" name="Remarks" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{37822F84-BE51-440E-9E33-7057374B8388}" name="Spalte1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7531F48-F369-427D-BF0E-B373BD3D9464}" name="Tabelle2" displayName="Tabelle2" ref="A16:D21" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7531F48-F369-427D-BF0E-B373BD3D9464}" name="Tabelle2" displayName="Tabelle2" ref="A16:D21" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A16:D21" xr:uid="{5C48C029-3835-4A93-A46E-44532C92FAA3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0447BFA7-3026-4AF7-A1B7-18AE0CFBF124}" name="UC" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A2FB336A-5D1A-465E-8C03-AD6268938476}" name="FP" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{AB75E940-54C0-4B8B-9EA7-F80E0F712E4D}" name="Time Total (/wo warm-up)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E3D2115D-CD04-4BCA-BD7D-98B341DA5312}" name="Time/FP" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{0447BFA7-3026-4AF7-A1B7-18AE0CFBF124}" name="UC" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A2FB336A-5D1A-465E-8C03-AD6268938476}" name="FP" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{AB75E940-54C0-4B8B-9EA7-F80E0F712E4D}" name="Time Total (/wo warm-up)" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{E3D2115D-CD04-4BCA-BD7D-98B341DA5312}" name="Time/FP" dataDxfId="11">
       <calculatedColumnFormula>C17/B17</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1899,7 +1899,7 @@
     <tableColumn id="3" xr3:uid="{19E74BDF-4684-4720-8463-4DBCA47C7700}" name="Time (estimated)">
       <calculatedColumnFormula>0.2558*B24+9.3956</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{358D21C6-AD94-4623-A21C-E1FAE50C991D}" name="Time spent" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{358D21C6-AD94-4623-A21C-E1FAE50C991D}" name="Time spent" dataDxfId="10">
       <calculatedColumnFormula>F11</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2206,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142AC939-646A-4C14-B811-03896D9CEEB5}">
   <dimension ref="A2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,13 +2249,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2394,14 +2394,14 @@
         <v>28</v>
       </c>
       <c r="D10" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="19">
         <v>15</v>
       </c>
       <c r="F10" s="20">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10">
         <f>37.72*2</f>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="D14" s="22">
         <f>SUM(Tabelle1[Testing ])</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="22">
         <f>SUM(Tabelle1[Warm-Up time])</f>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="F14" s="23">
         <f>SUM(Tabelle1[Total])</f>
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -2612,11 +2612,11 @@
       </c>
       <c r="C20" s="5">
         <f>SUM(B10:D10)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="7">
         <f t="shared" si="2"/>
-        <v>0.45068928950159071</v>
+        <v>0.46394485683987274</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2629,11 +2629,11 @@
       </c>
       <c r="C21" s="12">
         <f>SUM(C17:C20)</f>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D21" s="13">
         <f t="shared" si="2"/>
-        <v>0.49779751459370408</v>
+        <v>0.50137879167711208</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2664,7 +2664,7 @@
         <v>20.221056000000001</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D28" si="3">F11</f>
+        <f t="shared" ref="D24:D26" si="3">F11</f>
         <v>74</v>
       </c>
     </row>
@@ -2732,7 +2732,7 @@
         <f>C27*Tabelle3[[#This Row],[FP]]</f>
         <v>141.27243999999999</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="24" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hand in documents for the final
</commit_message>
<xml_diff>
--- a/documentation/useCases/TimeEstimationUC.xlsx
+++ b/documentation/useCases/TimeEstimationUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\useCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DB501-B7EB-434F-92E7-02635D1A870E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DA77D8-A38A-438B-9648-15004DA30E41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D6EDA16-4B89-4577-9EB0-EC9A0FBF9E49}"/>
   </bookViews>
@@ -2206,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142AC939-646A-4C14-B811-03896D9CEEB5}">
   <dimension ref="A2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="19">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D12" s="19">
         <v>2</v>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="F12" s="20">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G12">
         <v>34.200000000000003</v>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="C14" s="22">
         <f>SUM(Tabelle1[Coding ])</f>
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D14" s="22">
         <f>SUM(Tabelle1[Testing ])</f>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="F14" s="23">
         <f>SUM(Tabelle1[Total])</f>
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="D27">
         <f>SUM(D24:D26)</f>
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>